<commit_message>
Add material/products orders and work order
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA3FF9B-0BCA-4525-B8A0-AAB8CE0DE536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97FEBAD-AB8C-4902-B755-7C640FB58681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="887" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,33 @@
     <sheet name="설비" sheetId="5" r:id="rId5"/>
     <sheet name="설비에러종류" sheetId="6" r:id="rId6"/>
     <sheet name="설비에러로그" sheetId="7" r:id="rId7"/>
-    <sheet name="주문" sheetId="8" r:id="rId8"/>
-    <sheet name="생산지시" sheetId="9" r:id="rId9"/>
-    <sheet name="생산이력" sheetId="10" r:id="rId10"/>
-    <sheet name="생산정보" sheetId="11" r:id="rId11"/>
-    <sheet name="품질검사정보" sheetId="12" r:id="rId12"/>
-    <sheet name="품목입출고" sheetId="13" r:id="rId13"/>
-    <sheet name="품목재고현황" sheetId="14" r:id="rId14"/>
-    <sheet name="창고" sheetId="15" r:id="rId15"/>
-    <sheet name="근무자" sheetId="16" r:id="rId16"/>
-    <sheet name="사용자" sheetId="17" r:id="rId17"/>
+    <sheet name="고객제품주문" sheetId="8" r:id="rId8"/>
+    <sheet name="자사자재발주" sheetId="18" r:id="rId9"/>
+    <sheet name="생산지시" sheetId="9" r:id="rId10"/>
+    <sheet name="생산이력" sheetId="10" r:id="rId11"/>
+    <sheet name="생산정보" sheetId="11" r:id="rId12"/>
+    <sheet name="품질검사정보" sheetId="12" r:id="rId13"/>
+    <sheet name="품목입출고" sheetId="13" r:id="rId14"/>
+    <sheet name="품목재고현황" sheetId="14" r:id="rId15"/>
+    <sheet name="창고" sheetId="15" r:id="rId16"/>
+    <sheet name="근무자" sheetId="16" r:id="rId17"/>
+    <sheet name="사용자" sheetId="17" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="501">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -917,9 +927,6 @@
     <t>근무시간</t>
   </si>
   <si>
-    <t>주문상태</t>
-  </si>
-  <si>
     <t>근무위치</t>
   </si>
   <si>
@@ -1205,9 +1212,6 @@
     <t>생산지시 테이블 (WORK_ORDER)</t>
   </si>
   <si>
-    <t>주문 테이블 (CUST_ORDER)</t>
-  </si>
-  <si>
     <t>품질검사정보 테이블 (QUALITY)</t>
   </si>
   <si>
@@ -1497,6 +1501,54 @@
   </si>
   <si>
     <t>미완료</t>
+  </si>
+  <si>
+    <t>고객 제품 주문 테이블 (CUST_ORDER)</t>
+  </si>
+  <si>
+    <t>자사 자재 발주 테이블 (OUR_ORDER)</t>
+  </si>
+  <si>
+    <t>납품상태</t>
+  </si>
+  <si>
+    <t>order_dt</t>
+  </si>
+  <si>
+    <t>입고</t>
+  </si>
+  <si>
+    <t>미입고</t>
+  </si>
+  <si>
+    <t>기본값=미입고</t>
+  </si>
+  <si>
+    <t>1. 자재는 주문이 이뤄진 후 24시간이 지나면 입고(납품사→해당 공장 외부 창고)가 완료되는 것으로 가정</t>
+  </si>
+  <si>
+    <t>2. item_cd와 cust_cd가 동일하므로 주문시 item_cd 값만 입력받음</t>
+  </si>
+  <si>
+    <t>기본값=now()</t>
+  </si>
+  <si>
+    <t>1. item_cd와 cust_cd가 동일하므로 주문시 cust_cd 값만 입력받음</t>
+  </si>
+  <si>
+    <t>생산지시상태</t>
+  </si>
+  <si>
+    <t>wo_status</t>
+  </si>
+  <si>
+    <t>기본값=미생성</t>
+  </si>
+  <si>
+    <t>생성</t>
+  </si>
+  <si>
+    <t>미생성</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1882,11 +1934,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2158,6 +2219,30 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2200,6 +2285,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2224,20 +2321,20 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2561,11 +2658,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="s">
-        <v>381</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
+      <c r="A1" s="105" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2645,79 +2742,439 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.19921875" customWidth="1"/>
+    <col min="10" max="10" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.09765625" customWidth="1"/>
+    <col min="12" max="12" width="7.69921875" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="24" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="10.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="131" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="132"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" s="133" t="s">
+        <v>496</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K3" s="133" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="38">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38">
+        <v>1</v>
+      </c>
+      <c r="C4" s="38">
+        <v>2</v>
+      </c>
+      <c r="D4" s="38">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>44430</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="14">
+        <v>44432</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="3">
+        <f>100*1.05</f>
+        <v>105</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="57" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38">
+        <v>2</v>
+      </c>
+      <c r="D5" s="38">
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>44433</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="14">
+        <v>44437</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="57" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="38">
+        <v>3</v>
+      </c>
+      <c r="B6" s="74">
+        <v>1</v>
+      </c>
+      <c r="C6" s="38">
+        <v>3</v>
+      </c>
+      <c r="D6" s="38">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44446</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="14">
+        <v>44452</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="3">
+        <f>300*1.05</f>
+        <v>315</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>484</v>
+      </c>
+      <c r="K6" s="134" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="74">
+        <v>2</v>
+      </c>
+      <c r="C7" s="38">
+        <v>1</v>
+      </c>
+      <c r="D7" s="38">
+        <v>4</v>
+      </c>
+      <c r="E7" s="14">
+        <v>44450</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="14">
+        <v>44454</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>484</v>
+      </c>
+      <c r="K7" s="134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="74">
+        <v>2</v>
+      </c>
+      <c r="C8" s="38">
+        <v>3</v>
+      </c>
+      <c r="D8" s="38">
+        <v>5</v>
+      </c>
+      <c r="E8" s="14">
+        <v>44450</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="14">
+        <v>44454</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>484</v>
+      </c>
+      <c r="K8" s="134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="97" t="s">
+        <v>483</v>
+      </c>
+      <c r="K9" s="97" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="J10" s="97" t="s">
+        <v>481</v>
+      </c>
+      <c r="K10" s="97" t="s">
+        <v>481</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.09765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
+      <c r="A1" s="121" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>133</v>
@@ -2726,10 +3183,10 @@
         <v>290</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>224</v>
@@ -2740,10 +3197,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -2798,11 +3255,11 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="74">
-        <v>1</v>
-      </c>
-      <c r="B6" s="38">
+      <c r="A6" s="38">
         <v>3</v>
+      </c>
+      <c r="B6" s="74">
+        <v>1</v>
       </c>
       <c r="C6" s="38">
         <v>3</v>
@@ -2819,14 +3276,14 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="74">
-        <v>2</v>
-      </c>
-      <c r="B7" s="38">
-        <v>1</v>
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="74">
+        <v>2</v>
       </c>
       <c r="C7" s="38">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -2840,14 +3297,14 @@
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A8" s="74">
-        <v>2</v>
-      </c>
-      <c r="B8" s="38">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="74">
+        <v>2</v>
+      </c>
+      <c r="C8" s="38">
         <v>3</v>
-      </c>
-      <c r="C8" s="38">
-        <v>5</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -2883,14 +3340,14 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
-        <v>75</v>
+      <c r="A11" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>73</v>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -2908,13 +3365,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:G15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2922,40 +3379,40 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="7.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.19921875" customWidth="1"/>
-    <col min="17" max="17" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.8984375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A1" s="111" t="s">
-        <v>391</v>
-      </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="112"/>
-      <c r="P1" s="112"/>
-      <c r="Q1" s="112"/>
-      <c r="R1" s="112"/>
+      <c r="A1" s="123" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2968,34 +3425,34 @@
         <v>228</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>342</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N2" s="53" t="s">
         <v>169</v>
@@ -3010,10 +3467,10 @@
         <v>53</v>
       </c>
       <c r="R2" s="54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="T2" s="58" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.4">
@@ -3033,43 +3490,43 @@
         <v>82</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N3" s="55" t="s">
+        <v>366</v>
+      </c>
+      <c r="O3" s="55" t="s">
         <v>367</v>
       </c>
-      <c r="O3" s="55" t="s">
-        <v>368</v>
-      </c>
       <c r="P3" s="55" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q3" s="55" t="s">
         <v>364</v>
       </c>
-      <c r="Q3" s="55" t="s">
+      <c r="R3" s="56" t="s">
         <v>365</v>
-      </c>
-      <c r="R3" s="56" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.4">
@@ -3086,7 +3543,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="84" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F4" s="3">
         <v>40.049999999999997</v>
@@ -3146,7 +3603,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="84" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3176,7 +3633,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="84" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -3206,7 +3663,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -3236,7 +3693,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -3299,40 +3756,40 @@
         <v>73</v>
       </c>
       <c r="F11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="K11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="L11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="M11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="N11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="O11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="P11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="Q11" s="49" t="s">
         <v>360</v>
-      </c>
-      <c r="J11" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="K11" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="L11" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="M11" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="N11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="O11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="P11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q11" s="49" t="s">
-        <v>361</v>
       </c>
       <c r="R11" s="49"/>
     </row>
@@ -3347,27 +3804,27 @@
         <v>86</v>
       </c>
       <c r="Q12" s="49" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.4">
       <c r="H13" s="61" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I13" s="61" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M13" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.4">
@@ -3378,39 +3835,39 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.4">
       <c r="F15" s="35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G15" s="35" t="s">
+        <v>331</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>329</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>329</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>325</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>323</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="O15" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="J15" s="35" t="s">
-        <v>330</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>330</v>
-      </c>
-      <c r="L15" s="35" t="s">
+      <c r="P15" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q15" s="49" t="s">
         <v>326</v>
-      </c>
-      <c r="M15" s="35" t="s">
-        <v>324</v>
-      </c>
-      <c r="N15" s="49" t="s">
-        <v>325</v>
-      </c>
-      <c r="O15" s="49" t="s">
-        <v>333</v>
-      </c>
-      <c r="P15" s="49" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q15" s="49" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="17" spans="5:19" x14ac:dyDescent="0.4">
       <c r="E17" s="65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F17" s="91">
         <v>40</v>
@@ -3453,7 +3910,7 @@
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.4">
       <c r="E18" s="68" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F18" s="92">
         <v>0.1</v>
@@ -3498,50 +3955,50 @@
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.4">
       <c r="E19" s="63" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N19" s="59"/>
       <c r="O19" s="59"/>
       <c r="P19" s="59"/>
       <c r="Q19" s="34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R19" s="59"/>
       <c r="S19" s="59"/>
     </row>
     <row r="20" spans="5:19" x14ac:dyDescent="0.4">
       <c r="E20" s="71" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="62" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I20" s="62" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q20" s="52" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="21" spans="5:19" x14ac:dyDescent="0.4">
       <c r="E21" s="71" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="64" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I21" s="64" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K21" s="35"/>
     </row>
@@ -3550,10 +4007,10 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="64" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I22" s="64" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="5:19" x14ac:dyDescent="0.4">
@@ -3569,7 +4026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:P24"/>
@@ -3594,22 +4051,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A1" s="114" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="116"/>
+      <c r="A1" s="126" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="128"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -3622,34 +4079,34 @@
         <v>228</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>183</v>
       </c>
       <c r="J2" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="K2" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>340</v>
-      </c>
       <c r="M2" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N2" s="20" t="s">
         <v>173</v>
@@ -3716,7 +4173,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="84" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>52</v>
@@ -3763,7 +4220,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="84" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
@@ -3789,7 +4246,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="84" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
@@ -3815,7 +4272,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="84" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -3841,7 +4298,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -3902,55 +4359,55 @@
         <v>73</v>
       </c>
       <c r="F11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="I11" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="J11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="K11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="L11" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="M11" s="49" t="s">
         <v>360</v>
-      </c>
-      <c r="J11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="K11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="L11" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="M11" s="49" t="s">
-        <v>361</v>
       </c>
       <c r="N11" s="27"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="F13" s="48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G13" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>323</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="K13" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="L13" s="49" t="s">
+        <v>329</v>
+      </c>
+      <c r="M13" s="49" t="s">
         <v>326</v>
-      </c>
-      <c r="I13" s="48" t="s">
-        <v>324</v>
-      </c>
-      <c r="J13" s="49" t="s">
-        <v>325</v>
-      </c>
-      <c r="K13" s="49" t="s">
-        <v>333</v>
-      </c>
-      <c r="L13" s="49" t="s">
-        <v>330</v>
-      </c>
-      <c r="M13" s="49" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
@@ -3965,10 +4422,10 @@
         <v>88</v>
       </c>
       <c r="L14" s="45" t="s">
+        <v>361</v>
+      </c>
+      <c r="M14" s="45" t="s">
         <v>362</v>
-      </c>
-      <c r="M14" s="45" t="s">
-        <v>363</v>
       </c>
       <c r="N14" s="5"/>
     </row>
@@ -3986,10 +4443,10 @@
         <v>13</v>
       </c>
       <c r="J15" s="49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K15" s="49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L15" s="49" t="s">
         <v>17</v>
@@ -3999,12 +4456,12 @@
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.4">
-      <c r="C17" s="113" t="s">
-        <v>359</v>
-      </c>
-      <c r="D17" s="113"/>
+      <c r="C17" s="125" t="s">
+        <v>358</v>
+      </c>
+      <c r="D17" s="125"/>
       <c r="E17" s="61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F17" s="96">
         <v>40</v>
@@ -4035,7 +4492,7 @@
       <c r="C18" s="61"/>
       <c r="D18" s="61"/>
       <c r="E18" s="61" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F18" s="96">
         <v>0.1</v>
@@ -4064,12 +4521,12 @@
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.4">
       <c r="M19" s="34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.4">
       <c r="M20" s="52" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.4">
@@ -4092,13 +4549,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4113,20 +4570,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
-        <v>394</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="107"/>
+      <c r="A1" s="113" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="115"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -4198,7 +4655,7 @@
         <v>23</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L3" s="20" t="s">
         <v>160</v>
@@ -4455,13 +4912,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4476,15 +4933,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="108" t="s">
-        <v>396</v>
-      </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="110"/>
+      <c r="A1" s="116" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="118"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -4526,7 +4983,7 @@
         <v>158</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>130</v>
@@ -5673,13 +6130,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5692,13 +6149,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
-        <v>392</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="107"/>
+      <c r="A1" s="113" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="115"/>
       <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -5738,10 +6195,10 @@
       <c r="G3" s="79"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A4" s="37">
-        <v>1</v>
-      </c>
-      <c r="B4" s="37">
+      <c r="A4" s="104">
+        <v>1</v>
+      </c>
+      <c r="B4" s="104">
         <v>1</v>
       </c>
       <c r="C4" s="33" t="s">
@@ -5751,17 +6208,17 @@
         <v>60</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A5" s="37">
-        <v>1</v>
-      </c>
-      <c r="B5" s="37">
+      <c r="A5" s="104">
+        <v>1</v>
+      </c>
+      <c r="B5" s="104">
         <v>2</v>
       </c>
       <c r="C5" s="33" t="s">
@@ -5771,10 +6228,10 @@
         <v>55</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G5" s="80" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -5791,10 +6248,10 @@
         <v>60</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G6" s="80" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -5811,10 +6268,10 @@
         <v>55</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G7" s="80" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -5831,10 +6288,10 @@
         <v>60</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G8" s="80" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -5851,10 +6308,10 @@
         <v>55</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G9" s="80" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -5871,10 +6328,10 @@
         <v>60</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G10" s="80" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -5891,17 +6348,17 @@
         <v>55</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G11" s="80" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A12" s="37">
-        <v>2</v>
-      </c>
-      <c r="B12" s="37">
+      <c r="A12" s="104">
+        <v>2</v>
+      </c>
+      <c r="B12" s="104">
         <v>9</v>
       </c>
       <c r="C12" s="33" t="s">
@@ -5911,17 +6368,17 @@
         <v>60</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A13" s="37">
-        <v>2</v>
-      </c>
-      <c r="B13" s="37">
+      <c r="A13" s="104">
+        <v>2</v>
+      </c>
+      <c r="B13" s="104">
         <v>10</v>
       </c>
       <c r="C13" s="33" t="s">
@@ -5931,10 +6388,10 @@
         <v>55</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G13" s="80" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -5951,10 +6408,10 @@
         <v>60</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G14" s="85" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -5971,10 +6428,10 @@
         <v>55</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -5991,10 +6448,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G16" s="85" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -6011,10 +6468,10 @@
         <v>55</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G17" s="85" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -6031,10 +6488,10 @@
         <v>60</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G18" s="85" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -6051,10 +6508,10 @@
         <v>55</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G19" s="85" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
@@ -6094,17 +6551,17 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6117,14 +6574,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="108" t="s">
-        <v>393</v>
-      </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="110"/>
+      <c r="A1" s="116" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="118"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -6134,16 +6591,16 @@
         <v>219</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D2" s="39" t="s">
         <v>292</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -6183,13 +6640,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -6200,7 +6657,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>36</v>
@@ -6209,13 +6666,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>54</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -6235,13 +6692,13 @@
         <v>3</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>59</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -6252,7 +6709,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>54</v>
@@ -6261,7 +6718,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -6281,7 +6738,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -6292,7 +6749,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>59</v>
@@ -6301,7 +6758,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -6321,7 +6778,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -6332,7 +6789,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>36</v>
@@ -6341,7 +6798,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -6361,7 +6818,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -6372,7 +6829,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>54</v>
@@ -6381,7 +6838,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -6401,7 +6858,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -6412,7 +6869,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>59</v>
@@ -6421,7 +6878,7 @@
         <v>12</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -6441,7 +6898,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -6452,7 +6909,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>36</v>
@@ -6461,7 +6918,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -6481,7 +6938,7 @@
         <v>15</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -6492,7 +6949,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D19" s="29" t="s">
         <v>54</v>
@@ -6501,7 +6958,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -6521,7 +6978,7 @@
         <v>17</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -6532,7 +6989,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>59</v>
@@ -6541,7 +6998,7 @@
         <v>18</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -6561,7 +7018,7 @@
         <v>19</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -6572,7 +7029,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>36</v>
@@ -6581,7 +7038,7 @@
         <v>20</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -6601,7 +7058,7 @@
         <v>21</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -6612,7 +7069,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>54</v>
@@ -6621,7 +7078,7 @@
         <v>22</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -6641,7 +7098,7 @@
         <v>23</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -6652,7 +7109,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>59</v>
@@ -6661,7 +7118,7 @@
         <v>24</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -6681,7 +7138,7 @@
         <v>25</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -6692,7 +7149,7 @@
         <v>5</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>36</v>
@@ -6701,7 +7158,7 @@
         <v>26</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -6721,7 +7178,7 @@
         <v>27</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -6732,7 +7189,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>54</v>
@@ -6741,7 +7198,7 @@
         <v>28</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -6761,7 +7218,7 @@
         <v>29</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
@@ -6772,7 +7229,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>59</v>
@@ -6781,7 +7238,7 @@
         <v>30</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -6801,7 +7258,7 @@
         <v>31</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -6812,7 +7269,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>36</v>
@@ -6821,7 +7278,7 @@
         <v>32</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
@@ -6841,7 +7298,7 @@
         <v>33</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -6852,7 +7309,7 @@
         <v>6</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>54</v>
@@ -6861,7 +7318,7 @@
         <v>34</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -6881,7 +7338,7 @@
         <v>35</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
@@ -6892,7 +7349,7 @@
         <v>6</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>59</v>
@@ -6901,7 +7358,7 @@
         <v>36</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -6925,7 +7382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EFA5EA-225C-4ADE-B55C-E039C8436314}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -6943,56 +7400,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="117" t="s">
-        <v>467</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
+      <c r="A1" s="129" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
+        <v>466</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>467</v>
+      </c>
+      <c r="C2" s="88" t="s">
         <v>468</v>
       </c>
-      <c r="B2" s="88" t="s">
-        <v>469</v>
-      </c>
-      <c r="C2" s="88" t="s">
-        <v>470</v>
-      </c>
       <c r="D2" s="88" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="88" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B3" s="88" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C3" s="90" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="89" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B4" s="57">
         <v>12345</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D4" s="72">
         <v>44448.336921296293</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G4" s="52"/>
       <c r="H4" s="52"/>
@@ -7002,13 +7459,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="57" t="s">
+        <v>473</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>474</v>
+      </c>
+      <c r="C5" s="57" t="s">
         <v>475</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>476</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>477</v>
       </c>
       <c r="D5" s="72">
         <v>44465.425497685188</v>
@@ -7035,7 +7492,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7045,14 +7502,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="97" t="s">
-        <v>382</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
+      <c r="A1" s="105" t="s">
+        <v>381</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7262,16 +7719,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="98" t="s">
-        <v>383</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
+      <c r="A1" s="106" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -8100,7 +8557,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A6" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -8118,25 +8575,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="101" t="s">
-        <v>384</v>
-      </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="103"/>
+      <c r="A1" s="109" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="110"/>
+      <c r="C1" s="110"/>
+      <c r="D1" s="110"/>
+      <c r="E1" s="110"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
+      <c r="K1" s="110"/>
+      <c r="L1" s="110"/>
+      <c r="M1" s="111"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>228</v>
@@ -8148,28 +8605,28 @@
         <v>61</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F2" s="39" t="s">
+        <v>331</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="J2" s="39" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="K2" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>326</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>324</v>
-      </c>
-      <c r="I2" s="39" t="s">
-        <v>325</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>333</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>330</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>327</v>
       </c>
       <c r="M2" s="39" t="s">
         <v>38</v>
@@ -8183,10 +8640,10 @@
         <v>226</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D3" s="86" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>18</v>
@@ -8482,28 +8939,28 @@
       <c r="C14" s="44"/>
       <c r="D14" s="80"/>
       <c r="E14" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="I14" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="J14" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="K14" s="49" t="s">
         <v>360</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="L14" s="49" t="s">
         <v>360</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="J14" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="K14" s="49" t="s">
-        <v>361</v>
-      </c>
-      <c r="L14" s="49" t="s">
-        <v>361</v>
       </c>
       <c r="M14" s="44"/>
     </row>
@@ -8543,16 +9000,16 @@
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
       <c r="E17" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F17" s="46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H17" s="46" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I17" s="47" t="s">
         <v>169</v>
@@ -8586,16 +9043,16 @@
         <v>13</v>
       </c>
       <c r="I18" s="49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J18" s="49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K18" s="49" t="s">
         <v>17</v>
       </c>
       <c r="L18" s="49" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="M18" s="44"/>
     </row>
@@ -8615,12 +9072,12 @@
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B20" s="100" t="s">
-        <v>359</v>
-      </c>
-      <c r="C20" s="100"/>
+      <c r="B20" s="108" t="s">
+        <v>358</v>
+      </c>
+      <c r="C20" s="108"/>
       <c r="D20" s="61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E20" s="48">
         <v>40</v>
@@ -8653,7 +9110,7 @@
       <c r="B21" s="61"/>
       <c r="C21" s="61"/>
       <c r="D21" s="61" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E21" s="48">
         <v>0.1</v>
@@ -8683,12 +9140,12 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="L22" s="34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="L23" s="52" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -8721,20 +9178,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="98" t="s">
-        <v>385</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="99"/>
-      <c r="I1" s="99"/>
-      <c r="J1" s="99"/>
-      <c r="K1" s="99"/>
-      <c r="L1" s="104"/>
+      <c r="A1" s="106" t="s">
+        <v>384</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="112"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -9626,7 +10083,7 @@
         <v>241</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H26" s="31">
         <v>30</v>
@@ -9806,7 +10263,7 @@
         <v>241</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H31" s="31">
         <v>30</v>
@@ -9978,13 +10435,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
-        <v>386</v>
-      </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="107"/>
+      <c r="A1" s="113" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="115"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -10003,7 +10460,7 @@
         <v>38</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
@@ -10011,7 +10468,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>152</v>
@@ -10023,7 +10480,7 @@
         <v>130</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
@@ -10230,17 +10687,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="108" t="s">
-        <v>387</v>
-      </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="110"/>
+      <c r="A1" s="116" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="118"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -10447,10 +10904,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -10464,23 +10921,25 @@
     <col min="7" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="120" t="s">
-        <v>389</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="119" t="s">
+        <v>485</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>282</v>
       </c>
@@ -10494,10 +10953,10 @@
         <v>228</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>71</v>
@@ -10505,19 +10964,22 @@
       <c r="H2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>293</v>
+      <c r="I2" s="39" t="s">
+        <v>487</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K2" s="133" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>92</v>
@@ -10529,22 +10991,25 @@
         <v>128</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+        <v>401</v>
+      </c>
+      <c r="K3" s="133" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -10576,8 +11041,11 @@
         <f>H4-G4</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4" s="57" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="38">
         <v>2</v>
       </c>
@@ -10609,8 +11077,11 @@
         <f>H5-G5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K5" s="57" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="38">
         <v>3</v>
       </c>
@@ -10639,8 +11110,11 @@
       <c r="J6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6" s="134" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="38">
         <v>4</v>
       </c>
@@ -10669,8 +11143,11 @@
       <c r="J7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K7" s="134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="38">
         <v>5</v>
       </c>
@@ -10699,8 +11176,11 @@
       <c r="J8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K8" s="134" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -10716,7 +11196,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -10726,13 +11206,13 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+        <v>318</v>
+      </c>
+      <c r="K10" s="97" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>73</v>
       </c>
@@ -10749,12 +11229,17 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="119" t="s">
-        <v>483</v>
-      </c>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I11" s="97" t="s">
+        <v>481</v>
+      </c>
+      <c r="J11" s="97" t="s">
+        <v>481</v>
+      </c>
+      <c r="K11" s="97" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -10765,7 +11250,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -10776,9 +11261,14 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" s="52" t="s">
+        <v>495</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10786,327 +11276,257 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:L11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C930073-207E-4C86-90FD-855B24ED80AE}">
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.19921875" customWidth="1"/>
-    <col min="10" max="10" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="23" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="10.19921875" customWidth="1"/>
+    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="121" t="s">
-        <v>388</v>
-      </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="122"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A1" s="120" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>216</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>282</v>
+        <v>228</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>214</v>
+        <v>294</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>482</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>220</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>488</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" s="38">
-        <v>1</v>
-      </c>
-      <c r="B4" s="38">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38">
-        <v>2</v>
-      </c>
-      <c r="D4" s="38">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>44430</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="14">
-        <v>44432</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="3">
-        <f>100*1.05</f>
-        <v>105</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A5" s="38">
-        <v>2</v>
-      </c>
-      <c r="B5" s="38">
-        <v>2</v>
-      </c>
-      <c r="C5" s="38">
-        <v>2</v>
-      </c>
-      <c r="D5" s="38">
-        <v>2</v>
-      </c>
-      <c r="E5" s="14">
-        <v>44433</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="14">
-        <v>44437</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="3">
-        <f>200*1.05</f>
-        <v>210</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A6" s="38">
+        <v>21</v>
+      </c>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4" s="84">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84">
+        <v>4</v>
+      </c>
+      <c r="C4" s="84">
+        <v>1</v>
+      </c>
+      <c r="D4" s="84">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>300</v>
+      </c>
+      <c r="F4" s="10">
+        <v>44469.521064814813</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5" s="84">
+        <v>2</v>
+      </c>
+      <c r="B5" s="84">
+        <v>5</v>
+      </c>
+      <c r="C5" s="84">
+        <v>1</v>
+      </c>
+      <c r="D5" s="84">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>600</v>
+      </c>
+      <c r="F5" s="10">
+        <v>44469.521064814813</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6" s="84">
         <v>3</v>
       </c>
-      <c r="B6" s="74">
-        <v>1</v>
-      </c>
-      <c r="C6" s="38">
-        <v>3</v>
-      </c>
-      <c r="D6" s="38">
-        <v>3</v>
-      </c>
-      <c r="E6" s="14">
-        <v>44446</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="14">
-        <v>44452</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="3">
-        <f>300*1.05</f>
-        <v>315</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="38">
+      <c r="B6" s="84">
+        <v>6</v>
+      </c>
+      <c r="C6" s="98">
+        <v>1</v>
+      </c>
+      <c r="D6" s="84">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>700</v>
+      </c>
+      <c r="F6" s="10">
+        <v>44469.521064814813</v>
+      </c>
+      <c r="G6" s="99" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7" s="84">
         <v>4</v>
       </c>
-      <c r="B7" s="74">
-        <v>2</v>
-      </c>
-      <c r="C7" s="38">
-        <v>1</v>
-      </c>
-      <c r="D7" s="38">
+      <c r="B7" s="84">
         <v>4</v>
       </c>
-      <c r="E7" s="14">
-        <v>44450</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="14">
-        <v>44454</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="3">
-        <f>200*1.05</f>
-        <v>210</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A8" s="38">
+      <c r="C7" s="98">
+        <v>2</v>
+      </c>
+      <c r="D7" s="84">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>500</v>
+      </c>
+      <c r="F7" s="10">
+        <v>44470.641435185185</v>
+      </c>
+      <c r="G7" s="99" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" s="84">
         <v>5</v>
       </c>
-      <c r="B8" s="74">
-        <v>2</v>
-      </c>
-      <c r="C8" s="38">
-        <v>3</v>
-      </c>
-      <c r="D8" s="38">
+      <c r="B8" s="84">
         <v>5</v>
       </c>
-      <c r="E8" s="14">
-        <v>44450</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="14">
-        <v>44454</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="3">
-        <f>200*1.05</f>
-        <v>210</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="119" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="J10" s="119" t="s">
-        <v>483</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A11" s="7" t="s">
+      <c r="C8" s="98">
+        <v>2</v>
+      </c>
+      <c r="D8" s="84">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>400</v>
+      </c>
+      <c r="F8" s="10">
+        <v>44470.641435185185</v>
+      </c>
+      <c r="G8" s="99" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="84">
+        <v>6</v>
+      </c>
+      <c r="B9" s="84">
+        <v>6</v>
+      </c>
+      <c r="C9" s="98">
+        <v>2</v>
+      </c>
+      <c r="D9" s="84">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>600</v>
+      </c>
+      <c r="F9" s="10">
+        <v>44470.641435185185</v>
+      </c>
+      <c r="G9" s="99" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="F12" s="103" t="s">
+        <v>494</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>491</v>
+      </c>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G13" s="100" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="102" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="52" t="s">
+        <v>493</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add production start / production data generation / quality data generation
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F0502E-516B-4286-B6F9-146463B22E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712B0C16-986A-4EDD-88B6-67D860BF9A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="504">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1497,9 +1497,6 @@
     <t>입고</t>
   </si>
   <si>
-    <t>미입고</t>
-  </si>
-  <si>
     <t>기본값=미입고</t>
   </si>
   <si>
@@ -1555,6 +1552,12 @@
   </si>
   <si>
     <t>← item_1의 경우</t>
+  </si>
+  <si>
+    <t>(기본값=1)</t>
+  </si>
+  <si>
+    <t>추가!</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2258,84 +2261,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2344,6 +2269,102 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2667,11 +2688,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="117" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2756,7 +2777,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2778,19 +2799,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="133" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2827,7 +2848,7 @@
         <v>271</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -3089,7 +3110,7 @@
       <c r="D11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="134" t="s">
+      <c r="E11" s="108" t="s">
         <v>75</v>
       </c>
       <c r="F11" s="4"/>
@@ -3111,34 +3132,35 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="126" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="135" t="s">
         <v>386</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="128"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="137"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>214</v>
       </c>
@@ -3148,29 +3170,32 @@
       <c r="C2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="115" t="s">
+        <v>226</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>212</v>
       </c>
@@ -3180,151 +3205,169 @@
       <c r="C3" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="116" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4" s="38">
-        <v>1</v>
-      </c>
-      <c r="B4" s="38">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
-        <v>44430.291666666664</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="84">
+        <v>1</v>
+      </c>
+      <c r="B4" s="84">
+        <v>1</v>
+      </c>
+      <c r="C4" s="84">
+        <v>2</v>
+      </c>
+      <c r="D4" s="84">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
       </c>
       <c r="F4" s="10">
-        <v>44432.958333333336</v>
-      </c>
-      <c r="G4" s="3">
+        <v>44430.291678240741</v>
+      </c>
+      <c r="G4" s="10">
+        <v>44432.932650462964</v>
+      </c>
+      <c r="H4" s="3">
         <f>100*1.05</f>
         <v>105</v>
       </c>
-      <c r="H4" s="15">
+      <c r="I4" s="15">
         <v>102</v>
       </c>
-      <c r="I4" s="15">
-        <f>G4-H4</f>
+      <c r="J4" s="15">
+        <f>H4-I4</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A5" s="38">
-        <v>2</v>
-      </c>
-      <c r="B5" s="38">
-        <v>2</v>
-      </c>
-      <c r="C5" s="38">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
-        <v>44433.625</v>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="84">
+        <v>2</v>
+      </c>
+      <c r="B5" s="84">
+        <v>2</v>
+      </c>
+      <c r="C5" s="84">
+        <v>2</v>
+      </c>
+      <c r="D5" s="84">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
       </c>
       <c r="F5" s="10">
-        <v>44438.291666666664</v>
-      </c>
-      <c r="G5" s="3">
+        <v>44433.625011574077</v>
+      </c>
+      <c r="G5" s="10">
+        <v>44438.23265046296</v>
+      </c>
+      <c r="H5" s="3">
         <f>200*1.05</f>
         <v>210</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I5" s="15">
         <v>207</v>
       </c>
-      <c r="I5" s="15">
-        <f>G5-H5</f>
+      <c r="J5" s="15">
+        <f>H5-I5</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A6" s="38">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" s="84">
         <v>3</v>
       </c>
-      <c r="B6" s="74">
-        <v>1</v>
-      </c>
-      <c r="C6" s="38">
+      <c r="B6" s="98">
+        <v>1</v>
+      </c>
+      <c r="C6" s="84">
         <v>3</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
-        <v>44446.958333333336</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="15"/>
+      <c r="D6" s="84">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>44446.958344907405</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A7" s="38">
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="84">
         <v>4</v>
       </c>
-      <c r="B7" s="74">
-        <v>2</v>
-      </c>
-      <c r="C7" s="38">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>44450.291666666664</v>
-      </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="15"/>
+      <c r="B7" s="98">
+        <v>2</v>
+      </c>
+      <c r="C7" s="84">
+        <v>1</v>
+      </c>
+      <c r="D7" s="84">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>44450.291678240741</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A8" s="38">
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="84">
         <v>5</v>
       </c>
-      <c r="B8" s="74">
-        <v>2</v>
-      </c>
-      <c r="C8" s="38">
+      <c r="B8" s="98">
+        <v>2</v>
+      </c>
+      <c r="C8" s="84">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="E8" s="10">
-        <v>44450.625</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="15"/>
+      <c r="D8" s="84">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10">
+        <v>44450.625011574077</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3334,8 +3377,9 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3345,8 +3389,9 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>73</v>
       </c>
@@ -3356,19 +3401,27 @@
       <c r="C11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="D14" s="48" t="s">
+        <v>503</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3377,7 +3430,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3401,27 +3454,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="129"/>
-      <c r="R1" s="129"/>
-      <c r="S1" s="129"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="138"/>
+      <c r="R1" s="138"/>
+      <c r="S1" s="138"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -3546,7 +3599,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -3609,7 +3662,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -3642,7 +3695,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -3675,7 +3728,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -3708,7 +3761,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -3901,7 +3954,7 @@
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B17" s="135"/>
+      <c r="B17" s="109"/>
       <c r="F17" s="65" t="s">
         <v>349</v>
       </c>
@@ -3945,7 +3998,7 @@
       <c r="T17" s="59"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B18" s="135"/>
+      <c r="B18" s="109"/>
       <c r="F18" s="68" t="s">
         <v>350</v>
       </c>
@@ -4092,23 +4145,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="139" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="131"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="140"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -4209,7 +4262,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -4259,7 +4312,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -4288,7 +4341,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -4317,7 +4370,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -4346,7 +4399,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4409,7 +4462,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="40" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B11" s="78" t="s">
         <v>75</v>
@@ -4524,7 +4577,7 @@
       </c>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.4">
-      <c r="E17" s="136"/>
+      <c r="E17" s="110"/>
       <c r="F17" s="61" t="s">
         <v>349</v>
       </c>
@@ -4552,8 +4605,8 @@
       <c r="N17" s="95">
         <v>1</v>
       </c>
-      <c r="O17" s="136" t="s">
-        <v>502</v>
+      <c r="O17" s="110" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.4">
@@ -4621,7 +4674,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4636,33 +4689,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="112"/>
+      <c r="B1" s="111" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="118"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="113"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>200</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>207</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>160</v>
@@ -4690,17 +4743,17 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="114" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>157</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>151</v>
@@ -4732,13 +4785,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="38">
+        <v>1</v>
+      </c>
+      <c r="C4" s="38">
         <v>4</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="D4" s="38">
-        <v>1</v>
       </c>
       <c r="E4" s="22">
         <v>44390.738703703704</v>
@@ -4771,13 +4824,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="38">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38">
         <v>6</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="D5" s="38">
-        <v>2</v>
       </c>
       <c r="E5" s="22">
         <v>44419.765416666669</v>
@@ -4809,16 +4862,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="38">
-        <v>1</v>
-      </c>
-      <c r="C6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="38">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="D6" s="38">
-        <v>3</v>
       </c>
       <c r="E6" s="22">
         <v>44432.693495370368</v>
@@ -4850,16 +4903,16 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="38">
-        <v>2</v>
-      </c>
-      <c r="C7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="38">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="38">
-        <v>4</v>
       </c>
       <c r="E7" s="22">
         <v>44433.753321759257</v>
@@ -4940,16 +4993,16 @@
       <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A10" s="19" t="s">
-        <v>75</v>
+      <c r="A10" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="25" t="s">
-        <v>73</v>
-      </c>
+      <c r="C10" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="30"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="19" t="s">
@@ -4970,9 +5023,6 @@
       <c r="L10" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
 </worksheet>
@@ -4999,15 +5049,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="128" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="121"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="130"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -6202,12 +6252,12 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.69921875" bestFit="1" customWidth="1"/>
@@ -6215,21 +6265,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="139" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="140"/>
       <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>225</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>69</v>
@@ -6243,11 +6293,11 @@
       <c r="G2" s="79"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>156</v>
@@ -6282,10 +6332,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="104">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="104">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>197</v>
@@ -6302,10 +6352,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>198</v>
@@ -6322,10 +6372,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="37">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>199</v>
@@ -6342,10 +6392,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>206</v>
@@ -6362,10 +6412,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B9" s="37">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>194</v>
@@ -6382,10 +6432,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10" s="37">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>193</v>
@@ -6402,10 +6452,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="37">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B11" s="37">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" s="33" t="s">
         <v>202</v>
@@ -6422,10 +6472,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="104">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B12" s="104">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>201</v>
@@ -6442,10 +6492,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="104">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B13" s="104">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>189</v>
@@ -6462,10 +6512,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="37">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B14" s="37">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>203</v>
@@ -6482,10 +6532,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="37">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B15" s="37">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>195</v>
@@ -6502,10 +6552,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="37">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B16" s="37">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>191</v>
@@ -6522,10 +6572,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="37">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B17" s="37">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>204</v>
@@ -6542,10 +6592,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="37">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B18" s="37">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>192</v>
@@ -6562,10 +6612,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="37">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B19" s="37">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>205</v>
@@ -6595,11 +6645,11 @@
       <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>75</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>73</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="26"/>
@@ -6626,8 +6676,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:F26"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6640,14 +6690,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="136" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="128"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7466,12 +7516,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="141" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
@@ -7568,14 +7618,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="117" t="s">
         <v>374</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7785,16 +7835,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="118" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -8622,8 +8672,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="L11" sqref="E11:L11"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -8641,21 +8691,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="121" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="113"/>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="114"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="123"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="39" t="s">
@@ -9138,10 +9188,10 @@
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="120" t="s">
         <v>351</v>
       </c>
-      <c r="C20" s="111"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="61" t="s">
         <v>349</v>
       </c>
@@ -9244,20 +9294,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="118" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="115"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -10430,7 +10480,7 @@
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="97" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K34" s="97" t="s">
         <v>281</v>
@@ -10504,13 +10554,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="125" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="127"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -10756,17 +10806,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="128" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="121"/>
+      <c r="B1" s="129"/>
+      <c r="C1" s="129"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="130"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -10994,19 +11044,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="131" t="s">
         <v>478</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -11040,7 +11090,7 @@
         <v>277</v>
       </c>
       <c r="K2" s="105" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -11075,7 +11125,7 @@
         <v>394</v>
       </c>
       <c r="K3" s="105" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -11111,7 +11161,7 @@
         <v>-1</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -11147,7 +11197,7 @@
         <v>2</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -11180,7 +11230,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -11213,7 +11263,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="106" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -11246,7 +11296,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="106" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -11278,7 +11328,7 @@
         <v>316</v>
       </c>
       <c r="K10" s="97" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -11332,7 +11382,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -11349,7 +11399,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11360,15 +11410,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="132" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -11483,7 +11533,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G6" s="99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -11506,7 +11556,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G7" s="99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -11529,7 +11579,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G8" s="99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -11552,7 +11602,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G9" s="99" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -11569,26 +11619,26 @@
         <v>75</v>
       </c>
       <c r="F12" s="103" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G12" s="101" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G13" s="100" t="s">
-        <v>474</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="102" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="52" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get material_item_io and material_item_stock work done
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712B0C16-986A-4EDD-88B6-67D860BF9A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F0E27-D352-4372-8B02-204EABFAE5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="887" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="506">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1558,6 +1558,12 @@
   </si>
   <si>
     <t>추가!</t>
+  </si>
+  <si>
+    <t>null?</t>
+  </si>
+  <si>
+    <t>cust_cd = 0 은 회사 내부 이동을 의미</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1661,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1728,8 +1734,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1812,17 +1824,6 @@
     <border diagonalUp="1" diagonalDown="1">
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1956,7 +1957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2103,16 +2104,16 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2134,28 +2135,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2183,7 +2184,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2201,25 +2202,25 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2246,22 +2247,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2288,6 +2289,18 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2300,16 +2313,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2330,40 +2346,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2688,11 +2701,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="121" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2777,7 +2790,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G4" sqref="G4:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2799,19 +2812,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="137" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -3134,8 +3147,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3147,18 +3160,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="139" t="s">
         <v>386</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="141"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -3384,7 +3397,9 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="48" t="s">
+        <v>504</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -3430,7 +3445,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3454,27 +3469,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="142" t="s">
         <v>382</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="138"/>
-      <c r="R1" s="138"/>
-      <c r="S1" s="138"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
+      <c r="O1" s="142"/>
+      <c r="P1" s="142"/>
+      <c r="Q1" s="142"/>
+      <c r="R1" s="142"/>
+      <c r="S1" s="142"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -4123,7 +4138,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4145,23 +4160,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="143" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="140"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
+      <c r="O1" s="144"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -4671,10 +4686,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4780,39 +4795,41 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A4" s="38">
-        <v>1</v>
-      </c>
-      <c r="B4" s="38">
-        <v>1</v>
-      </c>
-      <c r="C4" s="38">
+    <row r="4" spans="1:14" s="59" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="74">
+        <v>1</v>
+      </c>
+      <c r="B4" s="74">
+        <v>1</v>
+      </c>
+      <c r="C4" s="74">
         <v>4</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="120">
         <v>44390.738703703704</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="38">
-        <v>1</v>
-      </c>
-      <c r="H4" s="18" t="s">
+      <c r="G4" s="74">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="74">
         <v>5</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="18">
+      <c r="K4" s="74">
+        <v>0</v>
+      </c>
+      <c r="L4" s="30">
         <v>300</v>
       </c>
       <c r="N4" s="23" t="s">
@@ -4932,7 +4949,9 @@
       <c r="J7" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="38">
+        <v>0</v>
+      </c>
       <c r="L7" s="18">
         <v>150</v>
       </c>
@@ -5022,9 +5041,17 @@
       </c>
       <c r="L10" s="26"/>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="K12" s="52" t="s">
+        <v>505</v>
+      </c>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+    </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5034,7 +5061,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5049,15 +5076,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="133" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="130"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="135"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -6252,7 +6279,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6265,13 +6292,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="143" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="140"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="144"/>
       <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -6351,22 +6378,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A6" s="37">
+      <c r="A6" s="117">
         <v>3</v>
       </c>
-      <c r="B6" s="37">
-        <v>1</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="B6" s="117">
+        <v>1</v>
+      </c>
+      <c r="C6" s="118" t="s">
         <v>198</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="117" t="s">
         <v>452</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="119" t="s">
         <v>434</v>
       </c>
     </row>
@@ -6391,22 +6418,22 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8" s="37">
+      <c r="A8" s="117">
         <v>5</v>
       </c>
-      <c r="B8" s="37">
-        <v>1</v>
-      </c>
-      <c r="C8" s="33" t="s">
+      <c r="B8" s="117">
+        <v>1</v>
+      </c>
+      <c r="C8" s="118" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="117" t="s">
         <v>453</v>
       </c>
-      <c r="G8" s="80" t="s">
+      <c r="G8" s="119" t="s">
         <v>436</v>
       </c>
     </row>
@@ -6431,22 +6458,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10" s="37">
+      <c r="A10" s="117">
         <v>7</v>
       </c>
-      <c r="B10" s="37">
-        <v>1</v>
-      </c>
-      <c r="C10" s="33" t="s">
+      <c r="B10" s="117">
+        <v>1</v>
+      </c>
+      <c r="C10" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="117" t="s">
         <v>454</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="G10" s="119" t="s">
         <v>438</v>
       </c>
     </row>
@@ -6511,22 +6538,22 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A14" s="37">
+      <c r="A14" s="117">
         <v>11</v>
       </c>
-      <c r="B14" s="37">
-        <v>2</v>
-      </c>
-      <c r="C14" s="33" t="s">
+      <c r="B14" s="117">
+        <v>2</v>
+      </c>
+      <c r="C14" s="118" t="s">
         <v>203</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="117" t="s">
         <v>455</v>
       </c>
-      <c r="G14" s="85" t="s">
+      <c r="G14" s="119" t="s">
         <v>444</v>
       </c>
     </row>
@@ -6551,22 +6578,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" s="37">
+      <c r="A16" s="117">
         <v>13</v>
       </c>
-      <c r="B16" s="37">
-        <v>2</v>
-      </c>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="117">
+        <v>2</v>
+      </c>
+      <c r="C16" s="118" t="s">
         <v>191</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="117" t="s">
         <v>456</v>
       </c>
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="119" t="s">
         <v>446</v>
       </c>
     </row>
@@ -6591,22 +6618,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A18" s="37">
+      <c r="A18" s="117">
         <v>15</v>
       </c>
-      <c r="B18" s="37">
-        <v>2</v>
-      </c>
-      <c r="C18" s="33" t="s">
+      <c r="B18" s="117">
+        <v>2</v>
+      </c>
+      <c r="C18" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="117" t="s">
         <v>457</v>
       </c>
-      <c r="G18" s="85" t="s">
+      <c r="G18" s="119" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6677,7 +6704,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6690,14 +6717,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="140" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="141"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -6740,7 +6767,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="29">
+      <c r="A4" s="104">
         <v>1</v>
       </c>
       <c r="B4" s="37">
@@ -6792,7 +6819,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="29">
+      <c r="A6" s="104">
         <v>3</v>
       </c>
       <c r="B6" s="37">
@@ -6838,7 +6865,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="29">
+      <c r="A8" s="104">
         <v>5</v>
       </c>
       <c r="B8" s="37">
@@ -7494,7 +7521,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7516,12 +7543,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="145" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
@@ -7618,14 +7645,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="121" t="s">
         <v>374</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7835,16 +7862,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="122" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -8673,7 +8700,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -8691,21 +8718,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="125" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="123"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="127"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="39" t="s">
@@ -9188,10 +9215,10 @@
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B20" s="120" t="s">
+      <c r="B20" s="124" t="s">
         <v>351</v>
       </c>
-      <c r="C20" s="120"/>
+      <c r="C20" s="124"/>
       <c r="D20" s="61" t="s">
         <v>349</v>
       </c>
@@ -9280,12 +9307,12 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.8984375" customWidth="1"/>
     <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
@@ -9294,33 +9321,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="128" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="124"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="129"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>223</v>
@@ -9348,17 +9375,17 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>95</v>
@@ -9392,11 +9419,11 @@
       <c r="B4" s="37">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>227</v>
-      </c>
-      <c r="D4" s="37">
-        <v>1</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>246</v>
@@ -9423,16 +9450,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="37">
         <v>1</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="37">
+        <v>1</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>232</v>
-      </c>
-      <c r="D5" s="37">
-        <v>2</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>117</v>
@@ -9459,16 +9486,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="37">
         <v>1</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>229</v>
-      </c>
-      <c r="D6" s="37">
-        <v>3</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>115</v>
@@ -9495,16 +9522,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="37">
         <v>1</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="37">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>104</v>
-      </c>
-      <c r="D7" s="37">
-        <v>4</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>111</v>
@@ -9531,16 +9558,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B8" s="37">
         <v>1</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="D8" s="37">
-        <v>5</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>116</v>
@@ -9567,16 +9594,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B9" s="37">
-        <v>2</v>
-      </c>
-      <c r="C9" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="37">
+        <v>2</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>220</v>
-      </c>
-      <c r="D9" s="37">
-        <v>6</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>246</v>
@@ -9603,16 +9630,16 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10" s="37">
-        <v>2</v>
-      </c>
-      <c r="C10" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="37">
+        <v>2</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>233</v>
-      </c>
-      <c r="D10" s="37">
-        <v>7</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>117</v>
@@ -9639,16 +9666,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="37">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B11" s="37">
-        <v>2</v>
-      </c>
-      <c r="C11" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="37">
+        <v>2</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>234</v>
-      </c>
-      <c r="D11" s="37">
-        <v>8</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>115</v>
@@ -9675,16 +9702,16 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="37">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B12" s="37">
-        <v>2</v>
-      </c>
-      <c r="C12" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="37">
+        <v>2</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>107</v>
-      </c>
-      <c r="D12" s="37">
-        <v>9</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>111</v>
@@ -9711,16 +9738,16 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="37">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B13" s="37">
-        <v>2</v>
-      </c>
-      <c r="C13" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="37">
+        <v>2</v>
+      </c>
+      <c r="D13" s="29" t="s">
         <v>100</v>
-      </c>
-      <c r="D13" s="37">
-        <v>10</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>116</v>
@@ -9747,16 +9774,16 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="37">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14" s="37">
+        <v>1</v>
+      </c>
+      <c r="C14" s="37">
         <v>3</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="D14" s="29" t="s">
         <v>213</v>
-      </c>
-      <c r="D14" s="37">
-        <v>11</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>246</v>
@@ -9783,16 +9810,16 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="37">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B15" s="37">
+        <v>1</v>
+      </c>
+      <c r="C15" s="37">
         <v>3</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="D15" s="29" t="s">
         <v>230</v>
-      </c>
-      <c r="D15" s="37">
-        <v>12</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>117</v>
@@ -9821,16 +9848,16 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="37">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B16" s="37">
+        <v>1</v>
+      </c>
+      <c r="C16" s="37">
         <v>3</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="D16" s="29" t="s">
         <v>231</v>
-      </c>
-      <c r="D16" s="37">
-        <v>13</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>115</v>
@@ -9857,16 +9884,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="37">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B17" s="37">
+        <v>1</v>
+      </c>
+      <c r="C17" s="37">
         <v>3</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>106</v>
-      </c>
-      <c r="D17" s="37">
-        <v>14</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>111</v>
@@ -9893,16 +9920,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="37">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B18" s="37">
+        <v>1</v>
+      </c>
+      <c r="C18" s="37">
         <v>3</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="D18" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="D18" s="37">
-        <v>15</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>116</v>
@@ -9929,16 +9956,16 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="37">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B19" s="37">
+        <v>2</v>
+      </c>
+      <c r="C19" s="37">
         <v>4</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="D19" s="29" t="s">
         <v>221</v>
-      </c>
-      <c r="D19" s="37">
-        <v>16</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>246</v>
@@ -9965,16 +9992,16 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="37">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B20" s="37">
+        <v>2</v>
+      </c>
+      <c r="C20" s="37">
         <v>4</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="D20" s="29" t="s">
         <v>256</v>
-      </c>
-      <c r="D20" s="37">
-        <v>17</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>117</v>
@@ -10001,16 +10028,16 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="37">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B21" s="37">
+        <v>2</v>
+      </c>
+      <c r="C21" s="37">
         <v>4</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="D21" s="29" t="s">
         <v>259</v>
-      </c>
-      <c r="D21" s="37">
-        <v>18</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>115</v>
@@ -10037,16 +10064,16 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="37">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B22" s="37">
+        <v>2</v>
+      </c>
+      <c r="C22" s="37">
         <v>4</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="D22" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="D22" s="37">
-        <v>19</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>111</v>
@@ -10073,16 +10100,16 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="37">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B23" s="37">
+        <v>2</v>
+      </c>
+      <c r="C23" s="37">
         <v>4</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="D23" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="D23" s="37">
-        <v>20</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>116</v>
@@ -10109,16 +10136,16 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" s="37">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B24" s="37">
+        <v>2</v>
+      </c>
+      <c r="C24" s="37">
         <v>5</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="D24" s="29" t="s">
         <v>228</v>
-      </c>
-      <c r="D24" s="37">
-        <v>21</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>246</v>
@@ -10145,16 +10172,16 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="37">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B25" s="37">
+        <v>2</v>
+      </c>
+      <c r="C25" s="37">
         <v>5</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="D25" s="29" t="s">
         <v>238</v>
-      </c>
-      <c r="D25" s="37">
-        <v>22</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>117</v>
@@ -10181,16 +10208,16 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="37">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B26" s="37">
+        <v>2</v>
+      </c>
+      <c r="C26" s="37">
         <v>5</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="D26" s="29" t="s">
         <v>262</v>
-      </c>
-      <c r="D26" s="37">
-        <v>23</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>115</v>
@@ -10217,16 +10244,16 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="37">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B27" s="37">
+        <v>2</v>
+      </c>
+      <c r="C27" s="37">
         <v>5</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="D27" s="29" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" s="37">
-        <v>24</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>111</v>
@@ -10253,16 +10280,16 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="37">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B28" s="37">
+        <v>2</v>
+      </c>
+      <c r="C28" s="37">
         <v>5</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="D28" s="29" t="s">
         <v>108</v>
-      </c>
-      <c r="D28" s="37">
-        <v>25</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>116</v>
@@ -10289,16 +10316,16 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="37">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B29" s="37">
+        <v>2</v>
+      </c>
+      <c r="C29" s="37">
         <v>6</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="D29" s="29" t="s">
         <v>215</v>
-      </c>
-      <c r="D29" s="37">
-        <v>26</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>246</v>
@@ -10325,16 +10352,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="37">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B30" s="37">
+        <v>2</v>
+      </c>
+      <c r="C30" s="37">
         <v>6</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="D30" s="29" t="s">
         <v>254</v>
-      </c>
-      <c r="D30" s="37">
-        <v>27</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>117</v>
@@ -10361,16 +10388,16 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" s="37">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B31" s="37">
+        <v>2</v>
+      </c>
+      <c r="C31" s="37">
         <v>6</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="D31" s="29" t="s">
         <v>255</v>
-      </c>
-      <c r="D31" s="37">
-        <v>28</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>115</v>
@@ -10397,16 +10424,16 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" s="37">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B32" s="37">
+        <v>2</v>
+      </c>
+      <c r="C32" s="37">
         <v>6</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="D32" s="29" t="s">
         <v>113</v>
-      </c>
-      <c r="D32" s="37">
-        <v>29</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>111</v>
@@ -10433,16 +10460,16 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" s="37">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B33" s="37">
+        <v>2</v>
+      </c>
+      <c r="C33" s="37">
         <v>6</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="D33" s="29" t="s">
         <v>120</v>
-      </c>
-      <c r="D33" s="37">
-        <v>30</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>116</v>
@@ -10500,11 +10527,13 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="L35" s="97" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A36" s="8" t="s">
-        <v>75</v>
+      <c r="A36" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>75</v>
@@ -10512,8 +10541,8 @@
       <c r="C36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>73</v>
+      <c r="D36" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -10554,13 +10583,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="130" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="127"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="132"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -10806,17 +10835,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="133" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="130"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -11044,19 +11073,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="128" t="s">
         <v>478</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -11399,7 +11428,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11410,15 +11439,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="136" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Add item_io and item_stock for production
1. update work_order
2. update equipment run_time
3. register item_io for production in
4. update item_stock for production in
5. register item_io for production out
6. register item_stock for production out
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F0E27-D352-4372-8B02-204EABFAE5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC13F5C8-62A8-4DD2-B5B8-11ACD82CE786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="887" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="507">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1530,9 +1530,6 @@
     <t>1. 자재는 주문이 이뤄지는 즉시 입고(공급회사→해당 공장 외부 창고)가 완료되는 것으로 가정</t>
   </si>
   <si>
-    <t>기본값=true</t>
-  </si>
-  <si>
     <t>PK/FK</t>
   </si>
   <si>
@@ -1564,6 +1561,12 @@
   </si>
   <si>
     <t>cust_cd = 0 은 회사 내부 이동을 의미</t>
+  </si>
+  <si>
+    <t>내부</t>
+  </si>
+  <si>
+    <t>기본값=1</t>
   </si>
 </sst>
 </file>
@@ -2301,6 +2304,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2308,18 +2323,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2701,11 +2704,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="125" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2790,7 +2793,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3147,8 +3150,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3398,7 +3401,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="48" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -3428,7 +3431,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="D14" s="48" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -3445,7 +3448,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3614,7 +3617,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -3677,7 +3680,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -3710,7 +3713,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -3743,7 +3746,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -3776,7 +3779,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4277,7 +4280,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -4327,7 +4330,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -4356,7 +4359,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -4385,7 +4388,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -4414,7 +4417,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4477,7 +4480,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B11" s="78" t="s">
         <v>75</v>
@@ -4621,7 +4624,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="110" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.4">
@@ -4688,7 +4691,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -5043,7 +5046,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="K12" s="52" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
@@ -6279,7 +6282,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6373,7 +6376,7 @@
       <c r="E5" s="37" t="s">
         <v>450</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="100" t="s">
         <v>442</v>
       </c>
     </row>
@@ -6533,7 +6536,7 @@
       <c r="E13" s="37" t="s">
         <v>451</v>
       </c>
-      <c r="G13" s="80" t="s">
+      <c r="G13" s="100" t="s">
         <v>441</v>
       </c>
     </row>
@@ -7645,14 +7648,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="125" t="s">
         <v>374</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7862,16 +7865,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="126" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -8697,16 +8700,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.19921875" bestFit="1" customWidth="1"/>
@@ -8718,28 +8721,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="122"/>
+      <c r="B1" s="121" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="127"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="123"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="39" t="s">
         <v>343</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>226</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>65</v>
@@ -8776,11 +8779,11 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>224</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>331</v>
@@ -8817,64 +8820,46 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="86">
+        <v>0</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="D4" s="86">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="37">
+        <v>1</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="37">
-        <v>1</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="C5" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="37">
-        <v>1</v>
-      </c>
-      <c r="E4" s="42">
+      <c r="D5" s="37">
+        <v>1</v>
+      </c>
+      <c r="E5" s="42">
         <v>40</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F5" s="42">
         <v>30</v>
-      </c>
-      <c r="G4" s="42">
-        <v>0</v>
-      </c>
-      <c r="H4" s="42">
-        <v>0</v>
-      </c>
-      <c r="I4" s="42">
-        <v>0</v>
-      </c>
-      <c r="J4" s="42">
-        <v>0</v>
-      </c>
-      <c r="K4" s="42">
-        <v>5</v>
-      </c>
-      <c r="L4" s="42">
-        <v>1</v>
-      </c>
-      <c r="M4" s="43">
-        <v>44381.564120370371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A5" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="37">
-        <v>2</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>178</v>
-      </c>
-      <c r="D5" s="37">
-        <v>2</v>
-      </c>
-      <c r="E5" s="42">
-        <v>30</v>
-      </c>
-      <c r="F5" s="42">
-        <v>20</v>
       </c>
       <c r="G5" s="42">
         <v>0</v>
@@ -8889,7 +8874,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" s="42">
         <v>1</v>
@@ -8899,23 +8884,23 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="37">
+        <v>2</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="37">
-        <v>3</v>
-      </c>
       <c r="C6" s="41" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D6" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="42">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F6" s="42">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G6" s="42">
         <v>0</v>
@@ -8930,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="42">
         <v>1</v>
@@ -8940,42 +8925,58 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="37">
+      <c r="A7" s="37">
+        <v>3</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="37">
+        <v>3</v>
+      </c>
+      <c r="E7" s="42">
+        <v>50</v>
+      </c>
+      <c r="F7" s="42">
+        <v>40</v>
+      </c>
+      <c r="G7" s="42">
+        <v>0</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0</v>
+      </c>
+      <c r="I7" s="42">
+        <v>0</v>
+      </c>
+      <c r="J7" s="42">
+        <v>0</v>
+      </c>
+      <c r="K7" s="42">
         <v>4</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="37">
-        <v>4</v>
-      </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="L7" s="42">
+        <v>1</v>
+      </c>
       <c r="M7" s="43">
         <v>44381.564120370371</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="37">
+        <v>4</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="37">
-        <v>5</v>
-      </c>
       <c r="C8" s="41" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="D8" s="37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
@@ -8990,17 +8991,17 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="37">
+        <v>5</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="37">
-        <v>6</v>
-      </c>
       <c r="C9" s="41" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D9" s="37">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
@@ -9015,19 +9016,29 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="44"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
+      <c r="A10" s="37">
+        <v>6</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="37">
+        <v>6</v>
+      </c>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43">
+        <v>44381.564120370371</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="44"/>
@@ -9076,50 +9087,50 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="44"/>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="48" t="s">
-        <v>352</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>352</v>
-      </c>
-      <c r="G14" s="48" t="s">
-        <v>352</v>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>352</v>
-      </c>
-      <c r="I14" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="J14" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="K14" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="L14" s="49" t="s">
-        <v>353</v>
-      </c>
-      <c r="M14" s="44"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="K15" s="49" t="s">
+        <v>353</v>
+      </c>
+      <c r="L15" s="49" t="s">
+        <v>353</v>
+      </c>
       <c r="M15" s="44"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
@@ -9142,30 +9153,14 @@
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
-      <c r="E17" s="46" t="s">
-        <v>300</v>
-      </c>
-      <c r="F17" s="46" t="s">
-        <v>298</v>
-      </c>
-      <c r="G17" s="46" t="s">
-        <v>335</v>
-      </c>
-      <c r="H17" s="46" t="s">
-        <v>326</v>
-      </c>
-      <c r="I17" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="K17" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" s="47" t="s">
-        <v>53</v>
-      </c>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
       <c r="M17" s="44"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
@@ -9173,129 +9168,155 @@
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="44"/>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="46" t="s">
+        <v>300</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="H18" s="46" t="s">
+        <v>326</v>
+      </c>
+      <c r="I18" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="K18" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="44"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F19" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="48" t="s">
+      <c r="H19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="49" t="s">
+      <c r="I19" s="49" t="s">
         <v>362</v>
       </c>
-      <c r="J18" s="49" t="s">
+      <c r="J19" s="49" t="s">
         <v>362</v>
       </c>
-      <c r="K18" s="49" t="s">
+      <c r="K19" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="49" t="s">
+      <c r="L19" s="49" t="s">
         <v>473</v>
       </c>
-      <c r="M18" s="44"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="35"/>
+      <c r="M19" s="44"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B20" s="124" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="35"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C21" s="124" t="s">
         <v>351</v>
       </c>
-      <c r="C20" s="124"/>
-      <c r="D20" s="61" t="s">
+      <c r="D21" s="61" t="s">
         <v>349</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E21" s="48">
         <v>40</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F21" s="48">
         <v>30</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G21" s="48">
         <v>0</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H21" s="48">
         <v>0</v>
       </c>
-      <c r="I20" s="49">
+      <c r="I21" s="49">
         <v>0</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J21" s="49">
         <v>0</v>
       </c>
-      <c r="K20" s="49">
+      <c r="K21" s="49">
         <v>5</v>
       </c>
-      <c r="L20" s="49">
-        <v>1</v>
-      </c>
-      <c r="M20" s="35"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" s="61"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61" t="s">
+      <c r="L21" s="49">
+        <v>1</v>
+      </c>
+      <c r="M21" s="35"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="61"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61" t="s">
         <v>350</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E22" s="48">
         <v>0.1</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F22" s="48">
         <v>0.1</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G22" s="48">
         <v>0.05</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H22" s="48">
         <v>0.05</v>
       </c>
-      <c r="I21" s="49">
+      <c r="I22" s="49">
         <v>0.01</v>
       </c>
-      <c r="J21" s="49">
+      <c r="J22" s="49">
         <v>0.01</v>
       </c>
-      <c r="K21" s="49">
+      <c r="K22" s="49">
         <v>0.1</v>
       </c>
-      <c r="L21" s="49">
+      <c r="L22" s="49">
         <v>0.1</v>
       </c>
-      <c r="M21" s="35"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="L22" s="34" t="s">
+      <c r="M22" s="35"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="L23" s="34" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="L23" s="52" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="L24" s="52" t="s">
         <v>472</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A1:M1"/>
-  </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9307,7 +9328,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -10507,7 +10528,7 @@
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="97" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="K34" s="97" t="s">
         <v>281</v>
@@ -11055,7 +11076,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11657,7 +11678,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G13" s="100" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Add 'cust_order update' functionality
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC13F5C8-62A8-4DD2-B5B8-11ACD82CE786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6DC6F5-0031-49FC-977D-101A129241F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="887" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="508">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1230,9 +1230,6 @@
     <t>finished_date</t>
   </si>
   <si>
-    <t>delayed_date</t>
-  </si>
-  <si>
     <t>start_date</t>
   </si>
   <si>
@@ -1567,6 +1564,12 @@
   </si>
   <si>
     <t>기본값=1</t>
+  </si>
+  <si>
+    <t>delayed_days</t>
+  </si>
+  <si>
+    <t>이름 수정</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1580,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1660,6 +1663,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
     </font>
@@ -1960,7 +1970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2380,6 +2390,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2864,7 +2880,7 @@
         <v>271</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -2884,13 +2900,13 @@
         <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>140</v>
@@ -3007,7 +3023,7 @@
         <v>315</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -3043,7 +3059,7 @@
         <v>210</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -3079,7 +3095,7 @@
         <v>210</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -3094,7 +3110,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="97" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -3108,7 +3124,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="K10" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -3150,8 +3166,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3401,7 +3417,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="48" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -3431,7 +3447,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="D14" s="48" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -3617,7 +3633,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -3680,7 +3696,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -3713,7 +3729,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -3746,7 +3762,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -3779,7 +3795,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4095,7 +4111,7 @@
         <v>366</v>
       </c>
       <c r="R20" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.4">
@@ -4141,7 +4157,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4280,7 +4296,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -4330,7 +4346,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -4359,7 +4375,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -4388,7 +4404,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -4417,7 +4433,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4480,7 +4496,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="40" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B11" s="78" t="s">
         <v>75</v>
@@ -4624,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="110" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.4">
@@ -4664,7 +4680,7 @@
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.4">
       <c r="N20" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.4">
@@ -5046,7 +5062,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="K12" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
@@ -5129,7 +5145,7 @@
         <v>156</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>129</v>
@@ -6354,10 +6370,10 @@
         <v>60</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -6374,10 +6390,10 @@
         <v>55</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G5" s="100" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -6394,10 +6410,10 @@
         <v>60</v>
       </c>
       <c r="E6" s="117" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G6" s="119" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -6414,10 +6430,10 @@
         <v>55</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G7" s="80" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -6434,10 +6450,10 @@
         <v>60</v>
       </c>
       <c r="E8" s="117" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G8" s="119" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -6454,10 +6470,10 @@
         <v>55</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G9" s="80" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -6474,10 +6490,10 @@
         <v>60</v>
       </c>
       <c r="E10" s="117" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G10" s="119" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -6494,10 +6510,10 @@
         <v>55</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G11" s="80" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -6514,10 +6530,10 @@
         <v>60</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -6534,10 +6550,10 @@
         <v>55</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G13" s="100" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -6554,10 +6570,10 @@
         <v>60</v>
       </c>
       <c r="E14" s="117" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G14" s="119" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -6574,10 +6590,10 @@
         <v>55</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -6594,10 +6610,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="117" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G16" s="119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -6614,10 +6630,10 @@
         <v>55</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G17" s="85" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -6634,10 +6650,10 @@
         <v>60</v>
       </c>
       <c r="E18" s="117" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G18" s="119" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -6654,10 +6670,10 @@
         <v>55</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G19" s="85" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
@@ -6786,7 +6802,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>36</v>
@@ -6812,7 +6828,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>54</v>
@@ -6838,7 +6854,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>59</v>
@@ -6864,7 +6880,7 @@
         <v>54</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -6884,7 +6900,7 @@
         <v>59</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -6904,7 +6920,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -6924,7 +6940,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -6944,7 +6960,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -6964,7 +6980,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -6984,7 +7000,7 @@
         <v>54</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -7004,7 +7020,7 @@
         <v>59</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -7024,7 +7040,7 @@
         <v>59</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -7044,7 +7060,7 @@
         <v>36</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -7064,7 +7080,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -7084,7 +7100,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -7104,7 +7120,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -7124,7 +7140,7 @@
         <v>59</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -7144,7 +7160,7 @@
         <v>59</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -7164,7 +7180,7 @@
         <v>36</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -7184,7 +7200,7 @@
         <v>36</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -7204,7 +7220,7 @@
         <v>54</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -7224,7 +7240,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -7244,7 +7260,7 @@
         <v>59</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -7264,7 +7280,7 @@
         <v>59</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -7284,7 +7300,7 @@
         <v>36</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -7304,7 +7320,7 @@
         <v>36</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -7324,7 +7340,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -7344,7 +7360,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -7364,7 +7380,7 @@
         <v>59</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
@@ -7384,7 +7400,7 @@
         <v>59</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -7404,7 +7420,7 @@
         <v>36</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -7424,7 +7440,7 @@
         <v>36</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
@@ -7444,7 +7460,7 @@
         <v>54</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -7464,7 +7480,7 @@
         <v>54</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -7484,7 +7500,7 @@
         <v>59</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
@@ -7504,7 +7520,7 @@
         <v>59</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -7547,7 +7563,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="145" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B1" s="146"/>
       <c r="C1" s="146"/>
@@ -7555,47 +7571,47 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>459</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="C2" s="88" t="s">
         <v>460</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>461</v>
-      </c>
       <c r="D2" s="88" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="88" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="88" t="s">
         <v>462</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>463</v>
-      </c>
       <c r="C3" s="90" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3" s="90" t="s">
         <v>470</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="89" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B4" s="57">
         <v>12345</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D4" s="72">
         <v>44448.336921296293</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G4" s="52"/>
       <c r="H4" s="52"/>
@@ -7605,13 +7621,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="57" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="57" t="s">
         <v>466</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="C5" s="57" t="s">
         <v>467</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>468</v>
       </c>
       <c r="D5" s="72">
         <v>44465.425497685188</v>
@@ -8824,10 +8840,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D4" s="86">
         <v>0</v>
@@ -9221,7 +9237,7 @@
         <v>17</v>
       </c>
       <c r="L19" s="49" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M19" s="44"/>
     </row>
@@ -9313,7 +9329,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="L24" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -10528,7 +10544,7 @@
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="97" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K34" s="97" t="s">
         <v>281</v>
@@ -11075,8 +11091,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11089,13 +11105,13 @@
     <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="128" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -11125,7 +11141,7 @@
         <v>292</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>71</v>
@@ -11134,13 +11150,13 @@
         <v>74</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>277</v>
       </c>
       <c r="K2" s="105" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -11171,11 +11187,11 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>394</v>
+      <c r="J3" s="115" t="s">
+        <v>506</v>
       </c>
       <c r="K3" s="105" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -11200,18 +11216,18 @@
       <c r="G4" s="14">
         <v>44433</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="147">
         <v>44432</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="148">
         <f>H4-G4</f>
         <v>-1</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -11236,18 +11252,18 @@
       <c r="G5" s="14">
         <v>44438</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="147">
         <v>44440</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="148">
         <f>H5-G5</f>
         <v>2</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -11280,7 +11296,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="106" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -11313,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -11346,7 +11362,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -11378,7 +11394,7 @@
         <v>316</v>
       </c>
       <c r="K10" s="97" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -11399,13 +11415,13 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -11432,7 +11448,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
-        <v>486</v>
+        <v>485</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -11461,7 +11480,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="136" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -11487,10 +11506,10 @@
         <v>292</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -11510,7 +11529,7 @@
         <v>127</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -11537,7 +11556,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -11560,7 +11579,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -11583,7 +11602,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G6" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -11606,7 +11625,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G7" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -11629,7 +11648,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G8" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -11652,7 +11671,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G9" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -11669,26 +11688,26 @@
         <v>75</v>
       </c>
       <c r="F12" s="103" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G12" s="101" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G13" s="100" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="102" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="52" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 'update cust_order' functionality
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC13F5C8-62A8-4DD2-B5B8-11ACD82CE786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6DC6F5-0031-49FC-977D-101A129241F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="887" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="508">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1230,9 +1230,6 @@
     <t>finished_date</t>
   </si>
   <si>
-    <t>delayed_date</t>
-  </si>
-  <si>
     <t>start_date</t>
   </si>
   <si>
@@ -1567,6 +1564,12 @@
   </si>
   <si>
     <t>기본값=1</t>
+  </si>
+  <si>
+    <t>delayed_days</t>
+  </si>
+  <si>
+    <t>이름 수정</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1580,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1660,6 +1663,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
     </font>
@@ -1960,7 +1970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2380,6 +2390,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2864,7 +2880,7 @@
         <v>271</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
@@ -2884,13 +2900,13 @@
         <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>140</v>
@@ -3007,7 +3023,7 @@
         <v>315</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -3043,7 +3059,7 @@
         <v>210</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
@@ -3079,7 +3095,7 @@
         <v>210</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -3094,7 +3110,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="97" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -3108,7 +3124,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="K10" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
@@ -3150,8 +3166,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3401,7 +3417,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="48" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -3431,7 +3447,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="D14" s="48" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -3617,7 +3633,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -3680,7 +3696,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -3713,7 +3729,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -3746,7 +3762,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -3779,7 +3795,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4095,7 +4111,7 @@
         <v>366</v>
       </c>
       <c r="R20" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.4">
@@ -4141,7 +4157,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4280,7 +4296,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="84" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B4" s="84">
         <v>1</v>
@@ -4330,7 +4346,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="84" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B5" s="84">
         <v>1</v>
@@ -4359,7 +4375,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="84" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B6" s="84">
         <v>1</v>
@@ -4388,7 +4404,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="84" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B7" s="84">
         <v>1</v>
@@ -4417,7 +4433,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="84" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B8" s="84">
         <v>1</v>
@@ -4480,7 +4496,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="40" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B11" s="78" t="s">
         <v>75</v>
@@ -4624,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="110" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.4">
@@ -4664,7 +4680,7 @@
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.4">
       <c r="N20" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.4">
@@ -5046,7 +5062,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="K12" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L12" s="52"/>
       <c r="M12" s="52"/>
@@ -5129,7 +5145,7 @@
         <v>156</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>129</v>
@@ -6354,10 +6370,10 @@
         <v>60</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -6374,10 +6390,10 @@
         <v>55</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G5" s="100" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -6394,10 +6410,10 @@
         <v>60</v>
       </c>
       <c r="E6" s="117" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G6" s="119" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
@@ -6414,10 +6430,10 @@
         <v>55</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G7" s="80" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
@@ -6434,10 +6450,10 @@
         <v>60</v>
       </c>
       <c r="E8" s="117" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G8" s="119" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -6454,10 +6470,10 @@
         <v>55</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G9" s="80" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -6474,10 +6490,10 @@
         <v>60</v>
       </c>
       <c r="E10" s="117" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G10" s="119" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
@@ -6494,10 +6510,10 @@
         <v>55</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G11" s="80" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -6514,10 +6530,10 @@
         <v>60</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -6534,10 +6550,10 @@
         <v>55</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G13" s="100" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -6554,10 +6570,10 @@
         <v>60</v>
       </c>
       <c r="E14" s="117" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G14" s="119" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -6574,10 +6590,10 @@
         <v>55</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G15" s="85" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
@@ -6594,10 +6610,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="117" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G16" s="119" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -6614,10 +6630,10 @@
         <v>55</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G17" s="85" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -6634,10 +6650,10 @@
         <v>60</v>
       </c>
       <c r="E18" s="117" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G18" s="119" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
@@ -6654,10 +6670,10 @@
         <v>55</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G19" s="85" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
@@ -6786,7 +6802,7 @@
         <v>36</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>36</v>
@@ -6812,7 +6828,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>54</v>
@@ -6838,7 +6854,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>59</v>
@@ -6864,7 +6880,7 @@
         <v>54</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -6884,7 +6900,7 @@
         <v>59</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -6904,7 +6920,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -6924,7 +6940,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -6944,7 +6960,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -6964,7 +6980,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -6984,7 +7000,7 @@
         <v>54</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -7004,7 +7020,7 @@
         <v>59</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -7024,7 +7040,7 @@
         <v>59</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -7044,7 +7060,7 @@
         <v>36</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -7064,7 +7080,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -7084,7 +7100,7 @@
         <v>54</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -7104,7 +7120,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -7124,7 +7140,7 @@
         <v>59</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -7144,7 +7160,7 @@
         <v>59</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
@@ -7164,7 +7180,7 @@
         <v>36</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -7184,7 +7200,7 @@
         <v>36</v>
       </c>
       <c r="F23" s="37" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
@@ -7204,7 +7220,7 @@
         <v>54</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
@@ -7224,7 +7240,7 @@
         <v>54</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -7244,7 +7260,7 @@
         <v>59</v>
       </c>
       <c r="F26" s="37" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -7264,7 +7280,7 @@
         <v>59</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -7284,7 +7300,7 @@
         <v>36</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -7304,7 +7320,7 @@
         <v>36</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
@@ -7324,7 +7340,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -7344,7 +7360,7 @@
         <v>54</v>
       </c>
       <c r="F31" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
@@ -7364,7 +7380,7 @@
         <v>59</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.4">
@@ -7384,7 +7400,7 @@
         <v>59</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -7404,7 +7420,7 @@
         <v>36</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -7424,7 +7440,7 @@
         <v>36</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
@@ -7444,7 +7460,7 @@
         <v>54</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -7464,7 +7480,7 @@
         <v>54</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -7484,7 +7500,7 @@
         <v>59</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.4">
@@ -7504,7 +7520,7 @@
         <v>59</v>
       </c>
       <c r="F39" s="37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.4">
@@ -7547,7 +7563,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="145" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B1" s="146"/>
       <c r="C1" s="146"/>
@@ -7555,47 +7571,47 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="88" t="s">
         <v>459</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="C2" s="88" t="s">
         <v>460</v>
       </c>
-      <c r="C2" s="88" t="s">
-        <v>461</v>
-      </c>
       <c r="D2" s="88" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="88" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="88" t="s">
         <v>462</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>463</v>
-      </c>
       <c r="C3" s="90" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3" s="90" t="s">
         <v>470</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="89" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B4" s="57">
         <v>12345</v>
       </c>
       <c r="C4" s="57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D4" s="72">
         <v>44448.336921296293</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G4" s="52"/>
       <c r="H4" s="52"/>
@@ -7605,13 +7621,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="57" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="57" t="s">
         <v>466</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="C5" s="57" t="s">
         <v>467</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>468</v>
       </c>
       <c r="D5" s="72">
         <v>44465.425497685188</v>
@@ -8824,10 +8840,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D4" s="86">
         <v>0</v>
@@ -9221,7 +9237,7 @@
         <v>17</v>
       </c>
       <c r="L19" s="49" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M19" s="44"/>
     </row>
@@ -9313,7 +9329,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="L24" s="52" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -10528,7 +10544,7 @@
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="97" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K34" s="97" t="s">
         <v>281</v>
@@ -11075,8 +11091,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11089,13 +11105,13 @@
     <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="128" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -11125,7 +11141,7 @@
         <v>292</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>71</v>
@@ -11134,13 +11150,13 @@
         <v>74</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>277</v>
       </c>
       <c r="K2" s="105" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -11171,11 +11187,11 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>394</v>
+      <c r="J3" s="115" t="s">
+        <v>506</v>
       </c>
       <c r="K3" s="105" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -11200,18 +11216,18 @@
       <c r="G4" s="14">
         <v>44433</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="147">
         <v>44432</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="148">
         <f>H4-G4</f>
         <v>-1</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -11236,18 +11252,18 @@
       <c r="G5" s="14">
         <v>44438</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="147">
         <v>44440</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="148" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="148">
         <f>H5-G5</f>
         <v>2</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -11280,7 +11296,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="106" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -11313,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -11346,7 +11362,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -11378,7 +11394,7 @@
         <v>316</v>
       </c>
       <c r="K10" s="97" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -11399,13 +11415,13 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="K11" s="97" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -11432,7 +11448,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
-        <v>486</v>
+        <v>485</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -11461,7 +11480,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="136" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B1" s="128"/>
       <c r="C1" s="128"/>
@@ -11487,10 +11506,10 @@
         <v>292</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -11510,7 +11529,7 @@
         <v>127</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>21</v>
@@ -11537,7 +11556,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -11560,7 +11579,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -11583,7 +11602,7 @@
         <v>44469.521064814813</v>
       </c>
       <c r="G6" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -11606,7 +11625,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G7" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -11629,7 +11648,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G8" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -11652,7 +11671,7 @@
         <v>44470.641435185185</v>
       </c>
       <c r="G9" s="99" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -11669,26 +11688,26 @@
         <v>75</v>
       </c>
       <c r="F12" s="103" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G12" s="101" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="G13" s="100" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="102" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="52" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete all the processes
A to Z
</commit_message>
<xml_diff>
--- a/Description/MES - DB 테이블.xlsx
+++ b/Description/MES - DB 테이블.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TH_MES\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84238A24-D305-42FD-B244-CD4661708AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F682B5D-0907-4DDF-BF20-B718C290437B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="887" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="공장" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="설비에러로그" sheetId="7" r:id="rId7"/>
     <sheet name="고객제품주문" sheetId="8" r:id="rId8"/>
     <sheet name="자사자재발주" sheetId="18" r:id="rId9"/>
-    <sheet name="생산지시" sheetId="9" r:id="rId10"/>
-    <sheet name="생산이력" sheetId="10" r:id="rId11"/>
-    <sheet name="생산정보" sheetId="11" r:id="rId12"/>
-    <sheet name="품질검사정보" sheetId="12" r:id="rId13"/>
-    <sheet name="품목입출고" sheetId="13" r:id="rId14"/>
-    <sheet name="품목재고현황" sheetId="14" r:id="rId15"/>
-    <sheet name="창고" sheetId="15" r:id="rId16"/>
-    <sheet name="근무자" sheetId="16" r:id="rId17"/>
-    <sheet name="사용자" sheetId="17" r:id="rId18"/>
+    <sheet name="생산예약자재" sheetId="19" r:id="rId10"/>
+    <sheet name="생산지시" sheetId="9" r:id="rId11"/>
+    <sheet name="생산이력" sheetId="10" r:id="rId12"/>
+    <sheet name="생산정보" sheetId="11" r:id="rId13"/>
+    <sheet name="품질검사정보" sheetId="12" r:id="rId14"/>
+    <sheet name="품목입출고" sheetId="13" r:id="rId15"/>
+    <sheet name="품목재고현황" sheetId="14" r:id="rId16"/>
+    <sheet name="창고" sheetId="15" r:id="rId17"/>
+    <sheet name="근무자" sheetId="16" r:id="rId18"/>
+    <sheet name="사용자" sheetId="17" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="528">
   <si>
     <t>사용가능여부</t>
   </si>
@@ -1569,7 +1570,67 @@
     <t>delayed_days</t>
   </si>
   <si>
-    <t>이름 수정</t>
+    <t>item4_qty</t>
+  </si>
+  <si>
+    <t>item5_qty</t>
+  </si>
+  <si>
+    <t>item6_qty</t>
+  </si>
+  <si>
+    <t>생산계획수량</t>
+  </si>
+  <si>
+    <t>생산품목코드</t>
+  </si>
+  <si>
+    <t>자재1 예약수량</t>
+  </si>
+  <si>
+    <t>자재2 예약수량</t>
+  </si>
+  <si>
+    <t>자재3 예약수량</t>
+  </si>
+  <si>
+    <t>기본값=미사용</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>생산사용여부</t>
+  </si>
+  <si>
+    <t>미사용 = 0</t>
+  </si>
+  <si>
+    <t>사용 = 1</t>
+  </si>
+  <si>
+    <t>used_yn</t>
+  </si>
+  <si>
+    <t>제품별 자재 소모 비율</t>
+  </si>
+  <si>
+    <t>생산예약자재 테이블 (RESERVED_ITEM)</t>
+  </si>
+  <si>
+    <t>cust_order의 order_no</t>
+  </si>
+  <si>
+    <t>자재발주상태</t>
+  </si>
+  <si>
+    <t>ourorder_status</t>
+  </si>
+  <si>
+    <t>신규 추가!!!</t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1641,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1673,8 +1734,12 @@
       <name val="맑은 고딕"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1750,6 +1815,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1970,7 +2041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2332,6 +2403,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2368,6 +2454,18 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2396,6 +2494,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2720,11 +2825,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="132" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -2804,12 +2909,391 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89BB437A-9486-40AE-9D9C-058E669EE172}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.09765625" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.796875" style="81"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="144" t="s">
+        <v>523</v>
+      </c>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="145"/>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2" s="88" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>511</v>
+      </c>
+      <c r="D2" s="88" t="s">
+        <v>510</v>
+      </c>
+      <c r="E2" s="88" t="s">
+        <v>512</v>
+      </c>
+      <c r="F2" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="G2" s="127" t="s">
+        <v>514</v>
+      </c>
+      <c r="H2" s="88" t="s">
+        <v>518</v>
+      </c>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A3" s="128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="129" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="88" t="s">
+        <v>507</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>508</v>
+      </c>
+      <c r="G3" s="127" t="s">
+        <v>509</v>
+      </c>
+      <c r="H3" s="88" t="s">
+        <v>521</v>
+      </c>
+      <c r="I3" s="146" t="s">
+        <v>522</v>
+      </c>
+      <c r="J3" s="147"/>
+      <c r="K3" s="147"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="57">
+        <v>1</v>
+      </c>
+      <c r="B4" s="57">
+        <v>1</v>
+      </c>
+      <c r="C4" s="57">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <f>100*1.05</f>
+        <v>105</v>
+      </c>
+      <c r="E4" s="57">
+        <f>D4*I4</f>
+        <v>210</v>
+      </c>
+      <c r="F4" s="57">
+        <f>D4*J4</f>
+        <v>315</v>
+      </c>
+      <c r="G4" s="57">
+        <f>D4*K4</f>
+        <v>105</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>520</v>
+      </c>
+      <c r="I4" s="79">
+        <v>2</v>
+      </c>
+      <c r="J4" s="79">
+        <v>3</v>
+      </c>
+      <c r="K4" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" s="57">
+        <v>2</v>
+      </c>
+      <c r="B5" s="57">
+        <v>2</v>
+      </c>
+      <c r="C5" s="57">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="E5" s="57">
+        <f t="shared" ref="E5:E8" si="0">D5*I5</f>
+        <v>420</v>
+      </c>
+      <c r="F5" s="57">
+        <f t="shared" ref="F5:F8" si="1">D5*J5</f>
+        <v>630</v>
+      </c>
+      <c r="G5" s="57">
+        <f t="shared" ref="G5:G8" si="2">D5*K5</f>
+        <v>210</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>520</v>
+      </c>
+      <c r="I5" s="79">
+        <v>2</v>
+      </c>
+      <c r="J5" s="79">
+        <v>3</v>
+      </c>
+      <c r="K5" s="79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" s="57">
+        <v>3</v>
+      </c>
+      <c r="B6" s="57">
+        <v>1</v>
+      </c>
+      <c r="C6" s="57">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <f>300*1.05</f>
+        <v>315</v>
+      </c>
+      <c r="E6" s="57">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="F6" s="57">
+        <f t="shared" si="1"/>
+        <v>630</v>
+      </c>
+      <c r="G6" s="57">
+        <f t="shared" si="2"/>
+        <v>945</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>519</v>
+      </c>
+      <c r="I6" s="79">
+        <v>1</v>
+      </c>
+      <c r="J6" s="79">
+        <v>2</v>
+      </c>
+      <c r="K6" s="79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="57">
+        <v>4</v>
+      </c>
+      <c r="B7" s="57">
+        <v>2</v>
+      </c>
+      <c r="C7" s="57">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="E7" s="57">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="F7" s="57">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="G7" s="57">
+        <f t="shared" si="2"/>
+        <v>420</v>
+      </c>
+      <c r="H7" s="57" t="s">
+        <v>519</v>
+      </c>
+      <c r="I7" s="79">
+        <v>3</v>
+      </c>
+      <c r="J7" s="79">
+        <v>1</v>
+      </c>
+      <c r="K7" s="79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A8" s="57">
+        <v>5</v>
+      </c>
+      <c r="B8" s="57">
+        <v>2</v>
+      </c>
+      <c r="C8" s="57">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <f>200*1.05</f>
+        <v>210</v>
+      </c>
+      <c r="E8" s="57">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="F8" s="57">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="G8" s="57">
+        <f t="shared" si="2"/>
+        <v>630</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>519</v>
+      </c>
+      <c r="I8" s="79">
+        <v>1</v>
+      </c>
+      <c r="J8" s="79">
+        <v>2</v>
+      </c>
+      <c r="K8" s="79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="130"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="131" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="131" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="131" t="s">
+        <v>281</v>
+      </c>
+      <c r="G11" s="131" t="s">
+        <v>281</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="108" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>524</v>
+      </c>
+      <c r="D14" s="81"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I3:K3"/>
+  </mergeCells>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2831,19 +3315,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="148" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="140"/>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -3161,7 +3645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:L14"/>
@@ -3179,18 +3663,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="150" t="s">
         <v>386</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="143"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="151"/>
+      <c r="J1" s="152"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -3459,7 +3943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:U23"/>
@@ -3488,27 +3972,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="153" t="s">
         <v>382</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="144"/>
-      <c r="K1" s="144"/>
-      <c r="L1" s="144"/>
-      <c r="M1" s="144"/>
-      <c r="N1" s="144"/>
-      <c r="O1" s="144"/>
-      <c r="P1" s="144"/>
-      <c r="Q1" s="144"/>
-      <c r="R1" s="144"/>
-      <c r="S1" s="144"/>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
+      <c r="J1" s="153"/>
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="153"/>
+      <c r="O1" s="153"/>
+      <c r="P1" s="153"/>
+      <c r="Q1" s="153"/>
+      <c r="R1" s="153"/>
+      <c r="S1" s="153"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -4152,7 +4636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:Q24"/>
@@ -4179,23 +4663,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="154" t="s">
         <v>381</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="145"/>
-      <c r="L1" s="145"/>
-      <c r="M1" s="145"/>
-      <c r="N1" s="145"/>
-      <c r="O1" s="146"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
+      <c r="O1" s="155"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -4702,7 +5186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:N12"/>
@@ -5074,7 +5558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:G54"/>
@@ -5095,15 +5579,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="140" t="s">
         <v>387</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="142"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -6292,7 +6776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:G23"/>
@@ -6311,13 +6795,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="154" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="146"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="155"/>
       <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -6717,7 +7201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:I42"/>
@@ -6736,14 +7220,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="151" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="152"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7544,7 +8028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EFA5EA-225C-4ADE-B55C-E039C8436314}">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -7562,12 +8046,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="156" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="88" t="s">
@@ -7664,14 +8148,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -7881,16 +8365,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="133" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -9343,8 +9827,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9358,20 +9842,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="135" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="131"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="136"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -10620,13 +11104,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="132" t="s">
+      <c r="A1" s="137" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="134"/>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="139"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -10872,17 +11356,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="140" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
+      <c r="I1" s="142"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
@@ -11089,10 +11573,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="P25" sqref="P25:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11105,26 +11589,28 @@
     <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="130" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="149" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
+      <c r="J1" s="149"/>
+      <c r="K1" s="149"/>
+      <c r="L1" s="149"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>280</v>
       </c>
@@ -11158,8 +11644,11 @@
       <c r="K2" s="105" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L2" s="160" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
         <v>128</v>
       </c>
@@ -11187,14 +11676,17 @@
       <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="159" t="s">
         <v>506</v>
       </c>
       <c r="K3" s="105" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L3" s="160" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="38">
         <v>1</v>
       </c>
@@ -11229,8 +11721,11 @@
       <c r="K4" s="57" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L4" s="89" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="38">
         <v>2</v>
       </c>
@@ -11265,8 +11760,11 @@
       <c r="K5" s="57" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L5" s="89" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="38">
         <v>3</v>
       </c>
@@ -11298,8 +11796,11 @@
       <c r="K6" s="106" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L6" s="89" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="38">
         <v>4</v>
       </c>
@@ -11331,8 +11832,11 @@
       <c r="K7" s="106" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L7" s="89" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="38">
         <v>5</v>
       </c>
@@ -11364,24 +11868,28 @@
       <c r="K8" s="106" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L8" s="89" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="64" t="s">
         <v>276</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="64" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L9" s="52"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -11390,14 +11898,18 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="64" t="s">
         <v>316</v>
       </c>
-      <c r="K10" s="97" t="s">
+      <c r="J10" s="158"/>
+      <c r="K10" s="64" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L10" s="46" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
         <v>73</v>
       </c>
@@ -11414,17 +11926,20 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="64" t="s">
         <v>473</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="64" t="s">
         <v>473</v>
       </c>
-      <c r="K11" s="97" t="s">
+      <c r="K11" s="64" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L11" s="46" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -11435,7 +11950,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -11445,18 +11960,64 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L13" s="46" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="52" t="s">
         <v>485</v>
       </c>
-      <c r="J14" s="48" t="s">
-        <v>507</v>
+      <c r="J14" s="48"/>
+    </row>
+    <row r="25" spans="12:16" x14ac:dyDescent="0.4">
+      <c r="L25">
+        <v>100</v>
+      </c>
+      <c r="M25">
+        <v>132</v>
+      </c>
+      <c r="N25">
+        <v>-210</v>
+      </c>
+      <c r="P25">
+        <f>SUM(L25:N25)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="12:16" x14ac:dyDescent="0.4">
+      <c r="L26">
+        <v>100</v>
+      </c>
+      <c r="M26">
+        <v>247</v>
+      </c>
+      <c r="N26">
+        <v>-315</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ref="P26:P27" si="0">SUM(L26:N26)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="12:16" x14ac:dyDescent="0.4">
+      <c r="L27">
+        <v>100</v>
+      </c>
+      <c r="M27">
+        <v>16</v>
+      </c>
+      <c r="N27">
+        <v>-105</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11468,7 +12029,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -11479,15 +12040,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="143" t="s">
         <v>478</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">

</xml_diff>